<commit_message>
fix errors (sort for better excel visulization errors)
</commit_message>
<xml_diff>
--- a/data/hierarchy/changed_codes_social.xlsx
+++ b/data/hierarchy/changed_codes_social.xlsx
@@ -448,324 +448,324 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>per_si_allsi.cov_q3_tot</t>
+          <t>per_si_allsi.ben_q1_tot</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SI.COV.Q3.TOT</t>
+          <t>SI.BEN.Q1.TOT</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>per_si_allsi.cov_q2_tot</t>
+          <t>per_sa_allsa.ben_q1_tot</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SI.COV.Q2.TOT</t>
+          <t>SA.BEN.Q1.TOT</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>per_si_allsi.cov_pop_tot</t>
+          <t>per_lm_alllm.ben_q1_tot</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SI.COV.POP.TOT</t>
+          <t>LM.BEN.Q1.TOT</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>per_si_allsi.cov_q4_tot</t>
+          <t>per_allsp.ben_q1_tot</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SI.COV.Q4.TOT</t>
+          <t>SP.BEN.Q1.TOT</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>per_si_allsi.cov_q1_tot</t>
+          <t>per_allsp.adq_pop_tot</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SI.COV.Q1.TOT</t>
+          <t>SP.ADQ.POP.TOT</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>per_sa_allsa.cov_q1_tot</t>
+          <t>per_si_allsi.adq_pop_tot</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SA.COV.Q1.TOT</t>
+          <t>SI.ADQ.POP.TOT</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>per_si_allsi.cov_q5_tot</t>
+          <t>per_lm_alllm.adq_pop_tot</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SI.COV.Q5.TOT</t>
+          <t>LM.ADQ.POP.TOT</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>per_allsp.cov_pop_tot</t>
+          <t>per_sa_allsa.adq_pop_tot</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SP.COV.POP.TOT</t>
+          <t>SA.ADQ.POP.TOT</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>per_sa_allsa.cov_q5_tot</t>
+          <t>per_sa_allsa.cov_q2_tot</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SA.COV.Q5.TOT</t>
+          <t>SA.COV.Q2.TOT</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>per_sa_allsa.cov_q3_tot</t>
+          <t>per_lm_alllm.cov_q5_tot</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SA.COV.Q3.TOT</t>
+          <t>LM.COV.Q5.TOT</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>per_sa_allsa.cov_pop_tot</t>
+          <t>per_lm_alllm.cov_q1_tot</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SA.COV.POP.TOT</t>
+          <t>LM.COV.Q1.TOT</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>per_sa_allsa.cov_q4_tot</t>
+          <t>per_lm_alllm.cov_q4_tot</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SA.COV.Q4.TOT</t>
+          <t>LM.COV.Q4.TOT</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>per_lm_alllm.cov_q1_tot</t>
+          <t>per_sa_allsa.cov_q4_tot</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>LM.COV.Q1.TOT</t>
+          <t>SA.COV.Q4.TOT</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>per_allsp.adq_pop_tot</t>
+          <t>per_si_allsi.cov_pop_tot</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SP.ADQ.POP.TOT</t>
+          <t>SI.COV.POP.TOT</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>per_lm_alllm.cov_pop_tot</t>
+          <t>per_si_allsi.cov_q2_tot</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LM.COV.POP.TOT</t>
+          <t>SI.COV.Q2.TOT</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>per_lm_alllm.cov_q2_tot</t>
+          <t>per_si_allsi.cov_q3_tot</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LM.COV.Q2.TOT</t>
+          <t>SI.COV.Q3.TOT</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>per_lm_alllm.cov_q3_tot</t>
+          <t>per_si_allsi.cov_q4_tot</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LM.COV.Q3.TOT</t>
+          <t>SI.COV.Q4.TOT</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>per_lm_alllm.cov_q4_tot</t>
+          <t>per_si_allsi.cov_q1_tot</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LM.COV.Q4.TOT</t>
+          <t>SI.COV.Q1.TOT</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>per_sa_allsa.cov_q2_tot</t>
+          <t>per_sa_allsa.cov_q1_tot</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SA.COV.Q2.TOT</t>
+          <t>SA.COV.Q1.TOT</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>per_lm_alllm.cov_q5_tot</t>
+          <t>per_si_allsi.cov_q5_tot</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LM.COV.Q5.TOT</t>
+          <t>SI.COV.Q5.TOT</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>per_si_allsi.ben_q1_tot</t>
+          <t>per_allsp.cov_pop_tot</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SI.BEN.Q1.TOT</t>
+          <t>SP.COV.POP.TOT</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>per_lm_alllm.ben_q1_tot</t>
+          <t>per_sa_allsa.cov_q3_tot</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LM.BEN.Q1.TOT</t>
+          <t>SA.COV.Q3.TOT</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>per_sa_allsa.adq_pop_tot</t>
+          <t>per_sa_allsa.cov_pop_tot</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SA.ADQ.POP.TOT</t>
+          <t>SA.COV.POP.TOT</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>per_lm_alllm.adq_pop_tot</t>
+          <t>per_sa_allsa.cov_q5_tot</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LM.ADQ.POP.TOT</t>
+          <t>SA.COV.Q5.TOT</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>per_allsp.ben_q1_tot</t>
+          <t>per_lm_alllm.cov_q3_tot</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SP.BEN.Q1.TOT</t>
+          <t>LM.COV.Q3.TOT</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>per_si_allsi.adq_pop_tot</t>
+          <t>per_lm_alllm.cov_q2_tot</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>SI.ADQ.POP.TOT</t>
+          <t>LM.COV.Q2.TOT</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>per_sa_allsa.ben_q1_tot</t>
+          <t>per_lm_alllm.cov_pop_tot</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SA.BEN.Q1.TOT</t>
+          <t>LM.COV.POP.TOT</t>
         </is>
       </c>
     </row>

</xml_diff>